<commit_message>
Cleaned up test data & provider
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0601EE5D-8489-4810-844E-28219D3887D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0DC7291F-2C8E-4619-9BA8-ED134E0F6984}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Path</t>
   </si>
@@ -33,46 +33,22 @@
     <t>/about-nci/visit</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>ContentType</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>english</t>
-  </si>
-  <si>
     <t>Article</t>
   </si>
   <si>
-    <t>Visitor Information</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
     <t>/about-nci/overview</t>
   </si>
   <si>
-    <t>Aspectos generales y misión del Instituto Nacional del Cáncer</t>
-  </si>
-  <si>
     <t>/espanol/instituto/general</t>
   </si>
   <si>
-    <t>spanish</t>
-  </si>
-  <si>
     <t>/espanol/acerca-sitio/mapa-sitio</t>
-  </si>
-  <si>
-    <t>Mapa del sitio</t>
-  </si>
-  <si>
-    <t>NCI Overview</t>
   </si>
 </sst>
 </file>
@@ -439,88 +415,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added LandingPage test class
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0DC7291F-2C8E-4619-9BA8-ED134E0F6984}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1A91210-CAD0-45CC-898B-FD1DD433AF0B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="InnerPage" sheetId="1" r:id="rId1"/>
+    <sheet name="HomePage" sheetId="2" r:id="rId1"/>
+    <sheet name="InnerPage" sheetId="1" r:id="rId2"/>
+    <sheet name="LandingPage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Path</t>
   </si>
@@ -49,6 +51,27 @@
   </si>
   <si>
     <t>/espanol/acerca-sitio/mapa-sitio</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Site Home</t>
+  </si>
+  <si>
+    <t>Landing Page</t>
+  </si>
+  <si>
+    <t>/about-nci</t>
+  </si>
+  <si>
+    <t>/espanol/instituto</t>
+  </si>
+  <si>
+    <t>/news-events</t>
+  </si>
+  <si>
+    <t>/espanol/noticias</t>
   </si>
 </sst>
 </file>
@@ -414,11 +437,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD42D8F-74E6-491F-B8F9-06EDAD02E472}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +460,41 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -465,6 +523,66 @@
       </c>
       <c r="B5" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E71B17D-D04E-47CE-A0C2-34E1B4101D15}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made test asserts classes consistent
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1A91210-CAD0-45CC-898B-FD1DD433AF0B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{48DE3FC4-CB36-4C13-A3B2-E4029AAE7C04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Path</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>/espanol/noticias</t>
+  </si>
+  <si>
+    <t>/espanol</t>
+  </si>
+  <si>
+    <t>/sites/nano</t>
+  </si>
+  <si>
+    <t>Home/Landing Page</t>
   </si>
 </sst>
 </file>
@@ -438,16 +447,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD42D8F-74E6-491F-B8F9-06EDAD02E472}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,6 +473,22 @@
       </c>
       <c r="B2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -535,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E71B17D-D04E-47CE-A0C2-34E1B4101D15}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added PDQ page load tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D468248D-6826-400E-8E66-D605905597A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12756" windowHeight="2640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CTHPPage" sheetId="5" r:id="rId1"/>
     <sheet name="HomePage" sheetId="2" r:id="rId2"/>
     <sheet name="InnerPage" sheetId="1" r:id="rId3"/>
     <sheet name="LandingPage" sheetId="3" r:id="rId4"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId5"/>
+    <sheet name="PDQPage" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
+    <sheet name="TopicPage" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>Path</t>
   </si>
@@ -115,12 +118,45 @@
   </si>
   <si>
     <t>/types/lung/hp</t>
+  </si>
+  <si>
+    <t>/types/lung/hp/lung-prevention-pdq</t>
+  </si>
+  <si>
+    <t>/espanol/tipos/pulmon/pro/prevencion-pulmon-pdq</t>
+  </si>
+  <si>
+    <t>/types/lung/hp/lung-prevention-pdq#section/all</t>
+  </si>
+  <si>
+    <t>/types/lung/hp/lung-prevention-pdq#section/_16</t>
+  </si>
+  <si>
+    <t>/types/lung/hp/lung-prevention-pdq#link/_225_toc</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq</t>
+  </si>
+  <si>
+    <t>/about-cancer/screening/patient-screening-overview-pdq</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#section/all</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#section/_149</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#link/_8</t>
+  </si>
+  <si>
+    <t>PDQ Cancer Info Summary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,20 +516,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A15:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -509,7 +545,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -517,7 +553,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -525,7 +561,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -539,20 +575,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -568,7 +604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -576,7 +612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -590,20 +626,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -619,7 +655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -627,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -635,7 +671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -650,20 +686,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -679,7 +715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -687,7 +723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -695,7 +731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -710,20 +746,140 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14744-CC2D-4AE2-9979-BD0B9D0ED780}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58053F56-5046-4F09-9D47-7878A0E9847F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -739,7 +895,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -747,7 +903,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -755,7 +911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Added blog load analytics tests; cleaned up data
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D468248D-6826-400E-8E66-D605905597A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{00889E07-7E11-48E9-92F8-C904B125690D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CTHPPage" sheetId="5" r:id="rId1"/>
-    <sheet name="HomePage" sheetId="2" r:id="rId2"/>
-    <sheet name="InnerPage" sheetId="1" r:id="rId3"/>
-    <sheet name="LandingPage" sheetId="3" r:id="rId4"/>
-    <sheet name="PDQPage" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId7"/>
+    <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
+    <sheet name="BlogSeriesPage" sheetId="7" r:id="rId2"/>
+    <sheet name="CTHPPage" sheetId="5" r:id="rId3"/>
+    <sheet name="HomePage" sheetId="2" r:id="rId4"/>
+    <sheet name="InnerPage" sheetId="1" r:id="rId5"/>
+    <sheet name="LandingPage" sheetId="3" r:id="rId6"/>
+    <sheet name="PDQPage" sheetId="6" r:id="rId7"/>
+    <sheet name="TopicPage" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>Path</t>
   </si>
@@ -138,9 +139,6 @@
     <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq</t>
   </si>
   <si>
-    <t>/about-cancer/screening/patient-screening-overview-pdq</t>
-  </si>
-  <si>
     <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#section/all</t>
   </si>
   <si>
@@ -151,6 +149,33 @@
   </si>
   <si>
     <t>PDQ Cancer Info Summary</t>
+  </si>
+  <si>
+    <t>/news-events/cancer-currents-blog</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/temas-y-relatos-blog</t>
+  </si>
+  <si>
+    <t>/research/key-initiatives/ras/ras-central/blog</t>
+  </si>
+  <si>
+    <t>Blog Series</t>
+  </si>
+  <si>
+    <t>/news-events/cancer-currents-blog/2018/selumetinib-nf1-neurofibromas</t>
+  </si>
+  <si>
+    <t>Blog Post</t>
+  </si>
+  <si>
+    <t>/espanol/instituto/organizacion/salud-mundial/blog/2017/dia-mundial-investigacion</t>
+  </si>
+  <si>
+    <t>/about-nci/organization/cgh/blog/2017/cancer-research-day</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/temas-y-relatos-blog/2018/selumetinib-neurofibromas-nf1</t>
   </si>
 </sst>
 </file>
@@ -516,11 +541,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC941920-D2D7-425D-AAC9-2581B925B1AF}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58053F56-5046-4F09-9D47-7878A0E9847F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A15:A16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,12 +709,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,12 +760,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,12 +820,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,12 +880,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14744-CC2D-4AE2-9979-BD0B9D0ED780}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +907,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,7 +915,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -788,7 +923,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +931,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -804,7 +939,7 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +947,7 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -820,7 +955,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,7 +963,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -836,15 +971,7 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -853,24 +980,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58053F56-5046-4F09-9D47-7878A0E9847F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added DynamicListingPage_Test; removed unneeded config files
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{00889E07-7E11-48E9-92F8-C904B125690D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B87EFA99-ADE7-42F7-BA5F-4F464852817A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
     <sheet name="BlogSeriesPage" sheetId="7" r:id="rId2"/>
     <sheet name="CTHPPage" sheetId="5" r:id="rId3"/>
-    <sheet name="HomePage" sheetId="2" r:id="rId4"/>
-    <sheet name="InnerPage" sheetId="1" r:id="rId5"/>
-    <sheet name="LandingPage" sheetId="3" r:id="rId6"/>
-    <sheet name="PDQPage" sheetId="6" r:id="rId7"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId8"/>
+    <sheet name="DynamicListingPage" sheetId="9" r:id="rId4"/>
+    <sheet name="HomePage" sheetId="2" r:id="rId5"/>
+    <sheet name="InnerPage" sheetId="1" r:id="rId6"/>
+    <sheet name="LandingPage" sheetId="3" r:id="rId7"/>
+    <sheet name="PDQPage" sheetId="6" r:id="rId8"/>
+    <sheet name="TopicPage" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>Path</t>
   </si>
@@ -176,6 +177,33 @@
   </si>
   <si>
     <t>/espanol/noticias/temas-y-relatos-blog/2018/selumetinib-neurofibromas-nf1</t>
+  </si>
+  <si>
+    <t>Disease Listing Page</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer/treatment</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer/treatment/trastuzumab</t>
+  </si>
+  <si>
+    <t>Intervention Listing Page</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/intervention/trastuzumab</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/intervention/trastuzumab/treatment</t>
+  </si>
+  <si>
+    <t>Manual Listing Page</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/kidney-cancer</t>
   </si>
 </sst>
 </file>
@@ -655,7 +683,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,6 +738,81 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150F8A41-7261-4E53-BBD5-6BBEA8E99D53}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -760,7 +863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -820,7 +923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -880,11 +983,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14744-CC2D-4AE2-9979-BD0B9D0ED780}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -980,7 +1083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added DynamicListingPage test changes
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B87EFA99-ADE7-42F7-BA5F-4F464852817A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F2A5E82-80BA-475E-9B9B-12F5B3BA2FE6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -683,13 +683,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +822,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -933,7 +933,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Fixed CTS view test failures
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1A1D5C3F-1E72-43F6-9B7A-EA4DFEACBC14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E1EFF7E7-6AC6-46D7-8571-357C7E2D8881}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
   <si>
     <t>Path</t>
   </si>
@@ -221,9 +221,6 @@
     <t>/about-cancer/treatment/clinical-trials/search/v?t=C9145&amp;st=C7780&amp;stg=C7881&amp;a=55&amp;q=epigenomic&amp;loc=0&amp;tid=AOST10B5&amp;in=Ching+C.+Lau&amp;lo=Childrens+Oncology+Group&amp;rl=2&amp;id=NCI-2011-02840&amp;pn=1&amp;ni=10</t>
   </si>
   <si>
-    <t>/clinicaltrials/NCT03200340</t>
-  </si>
-  <si>
     <t>CTS View Page</t>
   </si>
   <si>
@@ -288,6 +285,12 @@
   </si>
   <si>
     <t>Advanced</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/search/v?id=NCT03200340&amp;r=1</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/search/v?id=NCI-2016-00402&amp;r=1</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2D9579-CB1E-4EE4-968D-EC3BEFE113A6}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1063,51 +1066,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1117,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01AC777-2BAA-4DDD-9616-08ECBC5FC987}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,15 +1141,15 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>82</v>
@@ -1154,46 +1157,57 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
-        <v>62</v>
-      </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1225,58 +1239,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1290,7 +1304,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed failing dictionarypage tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E1EFF7E7-6AC6-46D7-8571-357C7E2D8881}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7B2292B3-9F71-4534-A79C-FA6D0CC00C98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
   <si>
     <t>Path</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>/about-cancer/treatment/clinical-trials/search/v?id=NCI-2016-00402&amp;r=1</t>
+  </si>
+  <si>
+    <t>/espanol/publicaciones/diccionario/def/yin-y-yang</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01AC777-2BAA-4DDD-9616-08ECBC5FC987}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1217,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E2B4AE-FC4B-430F-8D43-76B5FBC9E609}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,42 +1258,50 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DynamicListing - added assertions & refactored common items
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{83241EFF-1766-46F3-A356-2AFA90C4D381}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D9ED1953-A9F6-4F60-85BD-9E60D58D5E21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
@@ -181,9 +181,6 @@
     <t>/espanol/noticias/temas-y-relatos-blog/2018/selumetinib-neurofibromas-nf1</t>
   </si>
   <si>
-    <t>Disease Listing Page</t>
-  </si>
-  <si>
     <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer</t>
   </si>
   <si>
@@ -193,18 +190,12 @@
     <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer/treatment/trastuzumab</t>
   </si>
   <si>
-    <t>Intervention Listing Page</t>
-  </si>
-  <si>
     <t>/about-cancer/treatment/clinical-trials/intervention/trastuzumab</t>
   </si>
   <si>
     <t>/about-cancer/treatment/clinical-trials/intervention/trastuzumab/treatment</t>
   </si>
   <si>
-    <t>Manual Listing Page</t>
-  </si>
-  <si>
     <t>/about-cancer/treatment/clinical-trials/kidney-cancer</t>
   </si>
   <si>
@@ -278,6 +269,15 @@
   </si>
   <si>
     <t>/espanol/publicaciones/diccionario/def/yin-y-yang</t>
+  </si>
+  <si>
+    <t>Disease</t>
+  </si>
+  <si>
+    <t>Intervention</t>
+  </si>
+  <si>
+    <t>Manual</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC941920-D2D7-425D-AAC9-2581B925B1AF}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -993,73 +993,73 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1091,66 +1091,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1163,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150F8A41-7261-4E53-BBD5-6BBEA8E99D53}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,50 +1183,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DynamicListingPage_Test - added assertions
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D9ED1953-A9F6-4F60-85BD-9E60D58D5E21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C7CFE8CB-D4B4-4FDC-8EEF-9D2623D08C28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
   <si>
     <t>Path</t>
   </si>
@@ -278,6 +278,27 @@
   </si>
   <si>
     <t>Manual</t>
+  </si>
+  <si>
+    <t>ExpectedFilterInfo</t>
+  </si>
+  <si>
+    <t>disease|breast-cancer|none|none|</t>
+  </si>
+  <si>
+    <t>disease|breast-cancer|treatment|none|</t>
+  </si>
+  <si>
+    <t>disease|breast-cancer|treatment|trastuzumab|</t>
+  </si>
+  <si>
+    <t>intervention|trastuzumab|none|</t>
+  </si>
+  <si>
+    <t>intervention|trastuzumab|treatment|</t>
+  </si>
+  <si>
+    <t>manual parameters|</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1182,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150F8A41-7261-4E53-BBD5-6BBEA8E99D53}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -1171,62 +1192,84 @@
   <cols>
     <col min="1" max="1" width="80" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
       <c r="B7" t="s">
         <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PDQ data source
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C4799095-144A-4C3C-814F-91B8195B9D4C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{53889D78-889D-412B-985C-2EB6602EFE8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
@@ -21,8 +21,7 @@
     <sheet name="HomePage" sheetId="2" r:id="rId6"/>
     <sheet name="InnerPage" sheetId="1" r:id="rId7"/>
     <sheet name="LandingPage" sheetId="3" r:id="rId8"/>
-    <sheet name="PDQPage" sheetId="6" r:id="rId9"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId10"/>
+    <sheet name="TopicPage" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>Path</t>
   </si>
@@ -121,36 +120,6 @@
   </si>
   <si>
     <t>/types/lung/hp</t>
-  </si>
-  <si>
-    <t>/types/lung/hp/lung-prevention-pdq</t>
-  </si>
-  <si>
-    <t>/espanol/tipos/pulmon/pro/prevencion-pulmon-pdq</t>
-  </si>
-  <si>
-    <t>/types/lung/hp/lung-prevention-pdq#section/all</t>
-  </si>
-  <si>
-    <t>/types/lung/hp/lung-prevention-pdq#section/_16</t>
-  </si>
-  <si>
-    <t>/types/lung/hp/lung-prevention-pdq#link/_225_toc</t>
-  </si>
-  <si>
-    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq</t>
-  </si>
-  <si>
-    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#section/all</t>
-  </si>
-  <si>
-    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#section/_149</t>
-  </si>
-  <si>
-    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#link/_8</t>
-  </si>
-  <si>
-    <t>PDQ Cancer Info Summary</t>
   </si>
   <si>
     <t>/news-events/cancer-currents-blog</t>
@@ -633,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC941920-D2D7-425D-AAC9-2581B925B1AF}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -653,93 +622,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -771,26 +681,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -881,66 +791,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -972,73 +882,73 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1218,17 +1128,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14744-CC2D-4AE2-9979-BD0B9D0ED780}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1241,78 +1151,37 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed dictionary data source; Added popup tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{53889D78-889D-412B-985C-2EB6602EFE8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F8F6CF0-9EC5-440E-8B19-898ACABB68DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
     <sheet name="BlogSeriesPage" sheetId="7" r:id="rId2"/>
     <sheet name="CTHPPage" sheetId="5" r:id="rId3"/>
-    <sheet name="DictionaryPage" sheetId="11" r:id="rId4"/>
-    <sheet name="DynamicListingPage" sheetId="9" r:id="rId5"/>
-    <sheet name="HomePage" sheetId="2" r:id="rId6"/>
-    <sheet name="InnerPage" sheetId="1" r:id="rId7"/>
-    <sheet name="LandingPage" sheetId="3" r:id="rId8"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId9"/>
+    <sheet name="DynamicListingPage" sheetId="9" r:id="rId4"/>
+    <sheet name="HomePage" sheetId="2" r:id="rId5"/>
+    <sheet name="InnerPage" sheetId="1" r:id="rId6"/>
+    <sheet name="LandingPage" sheetId="3" r:id="rId7"/>
+    <sheet name="TopicPage" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>Path</t>
   </si>
@@ -165,45 +164,6 @@
   </si>
   <si>
     <t>/about-cancer/treatment/clinical-trials/kidney-cancer</t>
-  </si>
-  <si>
-    <t>/publications/dictionaries/cancer-terms</t>
-  </si>
-  <si>
-    <t>/espanol/publicaciones/diccionario</t>
-  </si>
-  <si>
-    <t>/publications/dictionaries/cancer-drug</t>
-  </si>
-  <si>
-    <t>/publications/dictionaries/genetics-dictionary</t>
-  </si>
-  <si>
-    <t>/publications/dictionaries/cancer-terms?expand=D</t>
-  </si>
-  <si>
-    <t>/publications/dictionaries/cancer-terms/def/cadmium</t>
-  </si>
-  <si>
-    <t>/publications/dictionaries/cancer-terms/search?contains=true&amp;q=breast</t>
-  </si>
-  <si>
-    <t>Term Dictionary</t>
-  </si>
-  <si>
-    <t>Drug Dictionary</t>
-  </si>
-  <si>
-    <t>Genetics Dictionary</t>
-  </si>
-  <si>
-    <t>Dictionary Search</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>/espanol/publicaciones/diccionario/def/yin-y-yang</t>
   </si>
   <si>
     <t>Disease</t>
@@ -768,102 +728,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E2B4AE-FC4B-430F-8D43-76B5FBC9E609}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150F8A41-7261-4E53-BBD5-6BBEA8E99D53}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -882,7 +750,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,10 +758,10 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,10 +769,10 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,10 +780,10 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,10 +791,10 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,10 +802,10 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,10 +813,10 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -956,7 +824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1007,7 +875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1067,7 +935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1127,11 +995,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated CTS data source
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{71A008D6-4F09-4519-B3AD-05B8C10D8A73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F0D5F57-3BA8-47A2-A0E6-67AA196B6502}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
     <sheet name="BlogSeriesPage" sheetId="7" r:id="rId2"/>
     <sheet name="CTHPPage" sheetId="5" r:id="rId3"/>
-    <sheet name="DynamicListingPage" sheetId="9" r:id="rId4"/>
-    <sheet name="ErrorPage" sheetId="10" r:id="rId5"/>
-    <sheet name="HomePage" sheetId="2" r:id="rId6"/>
-    <sheet name="InnerPage" sheetId="1" r:id="rId7"/>
-    <sheet name="LandingPage" sheetId="3" r:id="rId8"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId9"/>
+    <sheet name="ErrorPage" sheetId="10" r:id="rId4"/>
+    <sheet name="HomePage" sheetId="2" r:id="rId5"/>
+    <sheet name="InnerPage" sheetId="1" r:id="rId6"/>
+    <sheet name="LandingPage" sheetId="3" r:id="rId7"/>
+    <sheet name="TopicPage" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>Path</t>
   </si>
@@ -147,54 +146,6 @@
   </si>
   <si>
     <t>/espanol/noticias/temas-y-relatos-blog/2018/selumetinib-neurofibromas-nf1</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer/treatment</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer/treatment/trastuzumab</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/intervention/trastuzumab</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/intervention/trastuzumab/treatment</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/kidney-cancer</t>
-  </si>
-  <si>
-    <t>Disease</t>
-  </si>
-  <si>
-    <t>Intervention</t>
-  </si>
-  <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>ExpectedFilterInfo</t>
-  </si>
-  <si>
-    <t>disease|breast-cancer|none|none|</t>
-  </si>
-  <si>
-    <t>disease|breast-cancer|treatment|none|</t>
-  </si>
-  <si>
-    <t>disease|breast-cancer|treatment|trastuzumab|</t>
-  </si>
-  <si>
-    <t>intervention|trastuzumab|none|</t>
-  </si>
-  <si>
-    <t>intervention|trastuzumab|treatment|</t>
-  </si>
-  <si>
-    <t>manual parameters|</t>
   </si>
   <si>
     <t>Error Page</t>
@@ -581,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC941920-D2D7-425D-AAC9-2581B925B1AF}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -747,107 +698,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150F8A41-7261-4E53-BBD5-6BBEA8E99D53}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -867,26 +721,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -946,7 +800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1006,7 +860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1066,7 +920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Split out blog tests & data
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,19 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F0D5F57-3BA8-47A2-A0E6-67AA196B6502}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E7360808-470C-4DC3-9862-6D506CD8207B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BlogPostPage" sheetId="8" r:id="rId1"/>
-    <sheet name="BlogSeriesPage" sheetId="7" r:id="rId2"/>
-    <sheet name="CTHPPage" sheetId="5" r:id="rId3"/>
-    <sheet name="ErrorPage" sheetId="10" r:id="rId4"/>
-    <sheet name="HomePage" sheetId="2" r:id="rId5"/>
-    <sheet name="InnerPage" sheetId="1" r:id="rId6"/>
-    <sheet name="LandingPage" sheetId="3" r:id="rId7"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId8"/>
+    <sheet name="CTHPPage" sheetId="5" r:id="rId1"/>
+    <sheet name="ErrorPage" sheetId="10" r:id="rId2"/>
+    <sheet name="HomePage" sheetId="2" r:id="rId3"/>
+    <sheet name="InnerPage" sheetId="1" r:id="rId4"/>
+    <sheet name="LandingPage" sheetId="3" r:id="rId5"/>
+    <sheet name="TopicPage" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>Path</t>
   </si>
@@ -119,33 +117,6 @@
   </si>
   <si>
     <t>/types/lung/hp</t>
-  </si>
-  <si>
-    <t>/news-events/cancer-currents-blog</t>
-  </si>
-  <si>
-    <t>/espanol/noticias/temas-y-relatos-blog</t>
-  </si>
-  <si>
-    <t>/research/key-initiatives/ras/ras-central/blog</t>
-  </si>
-  <si>
-    <t>Blog Series</t>
-  </si>
-  <si>
-    <t>/news-events/cancer-currents-blog/2018/selumetinib-nf1-neurofibromas</t>
-  </si>
-  <si>
-    <t>Blog Post</t>
-  </si>
-  <si>
-    <t>/espanol/instituto/organizacion/salud-mundial/blog/2017/dia-mundial-investigacion</t>
-  </si>
-  <si>
-    <t>/about-nci/organization/cgh/blog/2017/cancer-research-day</t>
-  </si>
-  <si>
-    <t>/espanol/noticias/temas-y-relatos-blog/2018/selumetinib-neurofibromas-nf1</t>
   </si>
   <si>
     <t>Error Page</t>
@@ -529,20 +500,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC941920-D2D7-425D-AAC9-2581B925B1AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="78.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,36 +521,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -588,116 +559,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58053F56-5046-4F09-9D47-7878A0E9847F}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -705,13 +566,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,28 +580,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -757,13 +618,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -779,7 +640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -787,7 +648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -800,7 +661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -808,13 +669,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,7 +683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -830,7 +691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -838,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -846,7 +707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -860,7 +721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -868,13 +729,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -890,7 +751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -898,7 +759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -906,7 +767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -920,7 +781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -928,13 +789,13 @@
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -950,7 +811,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -958,7 +819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -966,7 +827,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Updated data source for CTHPs
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pageload.xlsx
+++ b/test-data/webanalytics-pageload.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E7360808-470C-4DC3-9862-6D506CD8207B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CBE6DE47-CF2F-472E-A282-A2ACDC104371}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CTHPPage" sheetId="5" r:id="rId1"/>
-    <sheet name="ErrorPage" sheetId="10" r:id="rId2"/>
-    <sheet name="HomePage" sheetId="2" r:id="rId3"/>
-    <sheet name="InnerPage" sheetId="1" r:id="rId4"/>
-    <sheet name="LandingPage" sheetId="3" r:id="rId5"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId6"/>
+    <sheet name="HomePage" sheetId="2" r:id="rId1"/>
+    <sheet name="InnerPage" sheetId="1" r:id="rId2"/>
+    <sheet name="LandingPage" sheetId="3" r:id="rId3"/>
+    <sheet name="TopicPage" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Path</t>
   </si>
@@ -99,42 +97,6 @@
   </si>
   <si>
     <t>Topic Page</t>
-  </si>
-  <si>
-    <t>CTHP HP</t>
-  </si>
-  <si>
-    <t>CTHP Patient</t>
-  </si>
-  <si>
-    <t>/espanol/tipos/piel</t>
-  </si>
-  <si>
-    <t>/espanol/tipos/piel/pro</t>
-  </si>
-  <si>
-    <t>/types/lung</t>
-  </si>
-  <si>
-    <t>/types/lung/hp</t>
-  </si>
-  <si>
-    <t>Error Page</t>
-  </si>
-  <si>
-    <t>Thank You</t>
-  </si>
-  <si>
-    <t>Page Not Found</t>
-  </si>
-  <si>
-    <t>/PublishedContent/ErrorMessages/Error.html</t>
-  </si>
-  <si>
-    <t>/PublishedContent/ErrorMessages/ThankYou.html</t>
-  </si>
-  <si>
-    <t>/PublishedContent/ErrorMessages/PageNotFound.html</t>
   </si>
 </sst>
 </file>
@@ -500,20 +462,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,36 +483,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -559,109 +513,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="51.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -669,13 +520,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -691,7 +542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -699,7 +550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -707,7 +558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -721,7 +572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -729,13 +580,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,7 +594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -751,7 +602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -759,7 +610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -767,7 +618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -781,7 +632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -789,13 +640,13 @@
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,7 +654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -811,7 +662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -819,7 +670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -827,7 +678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>

</xml_diff>